<commit_message>
Sync from DESKTOP-983I8EE - Sun 01/18/2026 16:55:20.32
</commit_message>
<xml_diff>
--- a/iterations.xlsx
+++ b/iterations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\code\FLL-Unearthed-2025---2026\Archive\final\Semi-Finals-(These files were working for the competition and now we will iterate only THESE files for the Semi-Finals)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\code\FLL-Unearthed-2025---2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33EA1CB6-47A2-477F-9E15-13D948CD9DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584289E-4E89-4ACC-A0EE-5481B803A24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="11">
   <si>
     <t>Run</t>
   </si>
@@ -60,11 +60,29 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>OLD MISSION</t>
+  </si>
+  <si>
+    <t>New Mission</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>mission pts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -258,11 +276,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -301,6 +328,30 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,19 +687,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BA3256-4EE1-4A5D-A5F4-1DDD101D2B98}">
-  <dimension ref="B1:O21"/>
+  <dimension ref="B1:AD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="235" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -691,8 +749,50 @@
       <c r="O2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>4</v>
+      </c>
+      <c r="V2" s="1">
+        <v>5</v>
+      </c>
+      <c r="W2" s="1">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -719,11 +819,33 @@
         <v>1</v>
       </c>
       <c r="O3" s="10">
-        <f>AVERAGE(C3:E3)</f>
+        <f t="shared" ref="O3:O10" si="0">AVERAGE(C3:E3)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="10" t="e">
+        <f>AVERAGE(S3:T3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -750,11 +872,32 @@
         <v>1</v>
       </c>
       <c r="O4" s="13">
-        <f>AVERAGE(C4:E4)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q4" s="3">
+        <v>2</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="13" t="e">
+        <f t="shared" ref="AD4:AD10" si="1">AVERAGE(R4:T4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -781,11 +924,32 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O5" s="13">
-        <f>AVERAGE(C5:E5)</f>
+        <f t="shared" si="0"/>
         <v>13.333333333333334</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q5" s="3">
+        <v>3</v>
+      </c>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -812,11 +976,36 @@
         <v>0</v>
       </c>
       <c r="O6" s="13">
-        <f>AVERAGE(C6:E6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" s="6">
+        <v>60</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6">
+        <v>60</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="13">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -843,11 +1032,32 @@
         <v>1</v>
       </c>
       <c r="O7" s="13">
-        <f>AVERAGE(C7:E7)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -874,11 +1084,32 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O8" s="13">
-        <f>AVERAGE(C8:E8)</f>
+        <f t="shared" si="0"/>
         <v>26.666666666666668</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q8" s="3">
+        <v>6</v>
+      </c>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -905,11 +1136,32 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O9" s="16">
-        <f>AVERAGE(C9:E9)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q9" s="8">
+        <v>7</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
@@ -936,16 +1188,40 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="O10" s="18">
-        <f>AVERAGE(C10:E10)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="11">
-        <v>46039</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -988,12 +1264,59 @@
       <c r="O13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>2</v>
+      </c>
+      <c r="T13" s="1">
+        <v>3</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>5</v>
+      </c>
+      <c r="W13" s="1">
+        <v>6</v>
+      </c>
+      <c r="X13" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="C14" s="22">
+        <v>60</v>
+      </c>
+      <c r="D14" s="20">
+        <v>10</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1008,17 +1331,48 @@
       <c r="N14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="O14" s="10" t="e">
+      <c r="O14" s="10">
         <f>AVERAGE(D14:E14)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="26">
+        <v>31.73</v>
+      </c>
+      <c r="S14" s="24">
+        <v>32.82</v>
+      </c>
+      <c r="T14" s="24"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7">
+        <v>60</v>
+      </c>
+      <c r="AC14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="10">
+        <f>AVERAGE(S14:T14)</f>
+        <v>32.82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="21">
+        <v>90</v>
+      </c>
+      <c r="D15" s="21">
+        <v>60</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1027,21 +1381,52 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="M15" s="6">
+        <v>120</v>
+      </c>
       <c r="N15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="13" t="e">
-        <f>AVERAGE(C15:E15)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="O15" s="13">
+        <f t="shared" ref="O15:O21" si="2">AVERAGE(C15:E15)</f>
+        <v>75</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>2</v>
+      </c>
+      <c r="R15" s="25">
+        <v>48.21</v>
+      </c>
+      <c r="S15" s="25">
+        <v>47.87</v>
+      </c>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD15" s="13">
+        <f t="shared" ref="AD15:AD21" si="3">AVERAGE(R15:T15)</f>
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="21">
+        <v>30</v>
+      </c>
+      <c r="D16" s="21">
+        <v>30</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1050,23 +1435,52 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="M16" s="6">
+        <v>60</v>
+      </c>
       <c r="N16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="13" t="e">
-        <f>AVERAGE(C16:E16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="O16" s="13">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3</v>
+      </c>
+      <c r="R16" s="25">
+        <v>61.98</v>
+      </c>
+      <c r="S16" s="25">
+        <v>53.54</v>
+      </c>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD16" s="13">
+        <f t="shared" si="3"/>
+        <v>57.76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C17" s="6">
-        <v>60</v>
-      </c>
-      <c r="D17" s="6"/>
+      <c r="C17" s="21">
+        <v>0</v>
+      </c>
+      <c r="D17" s="21">
+        <v>30</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -1076,22 +1490,53 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6">
+        <v>30</v>
+      </c>
+      <c r="N17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="13">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>4</v>
+      </c>
+      <c r="R17" s="25">
+        <v>25.09</v>
+      </c>
+      <c r="S17" s="25">
+        <v>23.33</v>
+      </c>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6">
         <v>60</v>
       </c>
-      <c r="N17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="O17" s="13">
-        <f>AVERAGE(C17:E17)</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="AC17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD17" s="13">
+        <f t="shared" si="3"/>
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>5</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="21">
+        <v>20</v>
+      </c>
+      <c r="D18" s="21">
+        <v>30</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1100,62 +1545,191 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="M18" s="6">
+        <v>100</v>
+      </c>
       <c r="N18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O18" s="13" t="e">
-        <f>AVERAGE(C18:E18)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="O18" s="13">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>5</v>
+      </c>
+      <c r="R18" s="25">
+        <v>18.05</v>
+      </c>
+      <c r="S18" s="25">
+        <v>20.22</v>
+      </c>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="13">
+        <f t="shared" si="3"/>
+        <v>19.134999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="N19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O19" s="13" t="e">
-        <f>AVERAGE(C19:E19)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q19" s="3">
+        <v>6</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="8">
         <v>7</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="N20" s="15" t="s">
         <v>5</v>
       </c>
       <c r="O20" s="16" t="e">
-        <f>AVERAGE(C20:E20)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q20" s="8">
+        <v>7</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="16" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1174,25 +1748,1087 @@
         <v>5</v>
       </c>
       <c r="O21" s="18" t="e">
-        <f>AVERAGE(C21:E21)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="Q21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD21" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="11">
+        <v>46040</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1">
+        <v>9</v>
+      </c>
+      <c r="L24" s="1">
+        <v>10</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>2</v>
+      </c>
+      <c r="T24" s="1">
+        <v>3</v>
+      </c>
+      <c r="U24" s="1">
+        <v>4</v>
+      </c>
+      <c r="V24" s="1">
+        <v>5</v>
+      </c>
+      <c r="W24" s="1">
+        <v>6</v>
+      </c>
+      <c r="X24" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7">
+        <v>60</v>
+      </c>
+      <c r="F25" s="7">
+        <v>50</v>
+      </c>
+      <c r="G25" s="7">
+        <v>50</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7">
+        <v>60</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" s="10">
+        <f>AVERAGE(D25:E25)</f>
+        <v>35</v>
+      </c>
+      <c r="P25" s="28">
+        <f>M25-O25</f>
+        <v>25</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>1</v>
+      </c>
+      <c r="R25" s="23">
+        <v>31.58</v>
+      </c>
+      <c r="S25" s="23">
+        <v>30.2</v>
+      </c>
+      <c r="T25" s="7">
+        <v>39.659999999999997</v>
+      </c>
+      <c r="U25" s="7">
+        <v>31.13</v>
+      </c>
+      <c r="V25" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7">
+        <v>60</v>
+      </c>
+      <c r="AC25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="10">
+        <f>AVERAGE(S25:T25)</f>
+        <v>34.93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>90</v>
+      </c>
+      <c r="D26">
+        <v>60</v>
+      </c>
+      <c r="E26" s="6">
+        <v>60</v>
+      </c>
+      <c r="F26" s="6">
+        <v>30</v>
+      </c>
+      <c r="G26" s="6">
+        <v>90</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6">
+        <v>120</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" ref="O26:O32" si="4">AVERAGE(C26:E26)</f>
+        <v>70</v>
+      </c>
+      <c r="P26" s="28">
+        <f t="shared" ref="P26:P29" si="5">M26-O26</f>
+        <v>50</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>2</v>
+      </c>
+      <c r="R26" s="23">
+        <v>42.4</v>
+      </c>
+      <c r="S26" s="23">
+        <v>37.44</v>
+      </c>
+      <c r="T26" s="6">
+        <v>27.12</v>
+      </c>
+      <c r="U26" s="6">
+        <v>27.24</v>
+      </c>
+      <c r="V26" s="6">
+        <v>25.73</v>
+      </c>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD26" s="13">
+        <f t="shared" ref="AD26:AD32" si="6">AVERAGE(R26:T26)</f>
+        <v>35.653333333333336</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
+        <v>60</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6">
+        <v>60</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="P27" s="28">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>3</v>
+      </c>
+      <c r="R27" s="23">
+        <v>37.42</v>
+      </c>
+      <c r="S27" s="23">
+        <v>39.729999999999997</v>
+      </c>
+      <c r="T27" s="6">
+        <v>38.46</v>
+      </c>
+      <c r="U27" s="6">
+        <v>43.48</v>
+      </c>
+      <c r="V27" s="6">
+        <v>36.130000000000003</v>
+      </c>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD27" s="13">
+        <f t="shared" si="6"/>
+        <v>38.536666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28" s="6">
+        <v>30</v>
+      </c>
+      <c r="F28" s="6">
+        <v>30</v>
+      </c>
+      <c r="G28" s="6">
+        <v>20</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6">
+        <v>30</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="4"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="P28" s="28">
+        <f t="shared" si="5"/>
+        <v>6.6666666666666679</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>4</v>
+      </c>
+      <c r="R28" s="23">
+        <v>31.58</v>
+      </c>
+      <c r="S28" s="23">
+        <v>26.84</v>
+      </c>
+      <c r="T28" s="6">
+        <v>23.75</v>
+      </c>
+      <c r="U28" s="6">
+        <v>38.92</v>
+      </c>
+      <c r="V28" s="6">
+        <v>25.52</v>
+      </c>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6">
+        <v>60</v>
+      </c>
+      <c r="AC28" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD28" s="13">
+        <f t="shared" si="6"/>
+        <v>27.39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="19">
+        <v>90</v>
+      </c>
+      <c r="D29" s="19">
+        <v>60</v>
+      </c>
+      <c r="E29" s="6">
+        <v>70</v>
+      </c>
+      <c r="F29" s="6">
+        <v>70</v>
+      </c>
+      <c r="G29" s="6">
+        <v>20</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6">
+        <v>100</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="4"/>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="P29" s="28">
+        <f t="shared" si="5"/>
+        <v>26.666666666666671</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>5</v>
+      </c>
+      <c r="R29" s="27">
+        <v>27.2</v>
+      </c>
+      <c r="S29" s="27">
+        <v>34.5</v>
+      </c>
+      <c r="T29" s="6">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="U29" s="6">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="V29" s="6">
+        <v>30.86</v>
+      </c>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD29" s="13">
+        <f t="shared" si="6"/>
+        <v>32.156666666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B30" s="3">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>6</v>
+      </c>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD30" s="13" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="8">
+        <v>7</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="O31" s="16" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>7</v>
+      </c>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD31" s="16" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <v>70</v>
+      </c>
+      <c r="F32" s="1">
+        <v>70</v>
+      </c>
+      <c r="G32" s="1">
+        <v>70</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O32" s="18">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD32" s="18" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1">
+        <v>6</v>
+      </c>
+      <c r="I35" s="1">
+        <v>7</v>
+      </c>
+      <c r="J35" s="1">
+        <v>8</v>
+      </c>
+      <c r="K35" s="1">
+        <v>9</v>
+      </c>
+      <c r="L35" s="1">
+        <v>10</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>1</v>
+      </c>
+      <c r="S35" s="1">
+        <v>2</v>
+      </c>
+      <c r="T35" s="1">
+        <v>3</v>
+      </c>
+      <c r="U35" s="1">
+        <v>4</v>
+      </c>
+      <c r="V35" s="1">
+        <v>5</v>
+      </c>
+      <c r="W35" s="1">
+        <v>6</v>
+      </c>
+      <c r="X35" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>9</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7">
+        <v>60</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O36" s="10" t="e">
+        <f>AVERAGE(D36:E36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>1</v>
+      </c>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7">
+        <v>60</v>
+      </c>
+      <c r="AC36" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD36" s="10" t="e">
+        <f>AVERAGE(S36:T36)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6">
+        <v>120</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O37" s="13" t="e">
+        <f t="shared" ref="O37:O43" si="7">AVERAGE(C37:E37)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>2</v>
+      </c>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="6"/>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6"/>
+      <c r="AC37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD37" s="13" t="e">
+        <f t="shared" ref="AD37:AD43" si="8">AVERAGE(R37:T37)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6">
+        <v>60</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" s="13" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>3</v>
+      </c>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="6"/>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+      <c r="AA38" s="6"/>
+      <c r="AB38" s="6"/>
+      <c r="AC38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD38" s="13" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>4</v>
+      </c>
+      <c r="C39" s="6">
+        <v>60</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6">
+        <v>30</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O39" s="13">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>4</v>
+      </c>
+      <c r="R39" s="6">
+        <v>60</v>
+      </c>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6">
+        <v>60</v>
+      </c>
+      <c r="AC39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD39" s="13">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B40" s="3">
+        <v>5</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6">
+        <v>100</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O40" s="13" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>5</v>
+      </c>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="6"/>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="6"/>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
+      <c r="AB40" s="6"/>
+      <c r="AC40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD40" s="13" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B41" s="3">
+        <v>6</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O41" s="13" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>6</v>
+      </c>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD41" s="13" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="8">
+        <v>7</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="O42" s="16" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>7</v>
+      </c>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="9"/>
+      <c r="Y42" s="9"/>
+      <c r="Z42" s="9"/>
+      <c r="AA42" s="9"/>
+      <c r="AB42" s="9"/>
+      <c r="AC42" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD42" s="16" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O43" s="18" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD43" s="18" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:M3 O3">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C3:M10 O3:O10">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:M3 O3">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1204,7 +2840,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:M4 O4">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1216,7 +2852,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M5 O5">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1228,7 +2864,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:M7 O7">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1240,7 +2876,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:M8 O8">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1252,7 +2888,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:M9 O9">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1264,7 +2912,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:M10 O10">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1276,6 +2924,220 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21 O21">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10:AB10 AD10">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10:AB10 AD10">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R21:AB21 AD21">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R21:AB21 AD21">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:M32 O32">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:M32 O32">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R32:AB32 AD32">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R32:AB32 AD32">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:M43 O43">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:M43 O43">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R43:AB43 AD43">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R43:AB43 AD43">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1287,7 +3149,55 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21 O21">
+  <conditionalFormatting sqref="C25:G29">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25:V29">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14:S18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:D18">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:M29">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1299,15 +3209,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
+  <conditionalFormatting sqref="P25:P29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Restore working tree to match 147aba7
</commit_message>
<xml_diff>
--- a/iterations.xlsx
+++ b/iterations.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\code\FLL-Unearthed-2025---2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarya\code\FLL-Unearthed-2025---2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB975B2A-545E-48B0-A801-294163E4D266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C727290-C3EE-459A-9FAA-AFB4486C509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="12960" windowHeight="7824" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Points" sheetId="1" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BEAFOOD">Points!$AGA$28</definedName>
-    <definedName name="BEAFOOD1">Points!$AGA$28</definedName>
-    <definedName name="lol">Points!$AGA$28</definedName>
+    <definedName name="BEAFOOD">Sheet1!$AGD$28</definedName>
+    <definedName name="BEAFOOD1">Sheet1!$AGD$28</definedName>
+    <definedName name="lol">Sheet1!$AGD$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="13">
   <si>
     <t>Run</t>
   </si>
@@ -62,11 +60,35 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>OLD MISSION</t>
+  </si>
+  <si>
+    <t>New Mission</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>mission pts</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Extension Setup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -260,11 +282,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -302,6 +390,56 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,19 +776,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BA3256-4EE1-4A5D-A5F4-1DDD101D2B98}">
-  <dimension ref="B1:O21"/>
+  <dimension ref="B1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="J13" zoomScale="63" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -693,8 +838,53 @@
       <c r="O2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="30"/>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1">
+        <v>3</v>
+      </c>
+      <c r="X2" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -724,8 +914,32 @@
         <f t="shared" ref="O3:O10" si="0">AVERAGE(C3:E3)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+      <c r="R3" s="31"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="10" t="e">
+        <f>AVERAGE(U3:W3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -755,8 +969,32 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q4" s="3">
+        <v>2</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="13" t="e">
+        <f>AVERAGE(S4:W4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -786,8 +1024,32 @@
         <f t="shared" si="0"/>
         <v>13.333333333333334</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q5" s="3">
+        <v>3</v>
+      </c>
+      <c r="R5" s="32"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG5" s="13" t="e">
+        <f>AVERAGE(S5:W5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -817,8 +1079,36 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q6" s="3">
+        <v>4</v>
+      </c>
+      <c r="R6" s="32"/>
+      <c r="S6" s="6">
+        <v>60</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6">
+        <v>60</v>
+      </c>
+      <c r="AF6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6" s="13">
+        <f>AVERAGE(S6:W6)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -848,8 +1138,32 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q7" s="3">
+        <v>5</v>
+      </c>
+      <c r="R7" s="32"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="13" t="e">
+        <f>AVERAGE(S7:W7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -879,8 +1193,32 @@
         <f t="shared" si="0"/>
         <v>26.666666666666668</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q8" s="3">
+        <v>6</v>
+      </c>
+      <c r="R8" s="32"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG8" s="13" t="e">
+        <f>AVERAGE(S8:W8)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -910,8 +1248,32 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q9" s="8">
+        <v>7</v>
+      </c>
+      <c r="R9" s="33"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG9" s="16" t="e">
+        <f>AVERAGE(S9:W9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
@@ -941,13 +1303,40 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="30"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="18" t="e">
+        <f>AVERAGE(S10:W10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
       <c r="D12" s="11">
-        <v>46039</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -990,12 +1379,62 @@
       <c r="O13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="Q13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="30"/>
+      <c r="S13" s="1">
+        <v>1</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1">
+        <v>2</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1">
+        <v>3</v>
+      </c>
+      <c r="X13" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="C14" s="22">
+        <v>60</v>
+      </c>
+      <c r="D14" s="20">
+        <v>10</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1010,17 +1449,51 @@
       <c r="N14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="O14" s="10" t="e">
+      <c r="O14" s="10">
         <f>AVERAGE(D14:E14)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>1</v>
+      </c>
+      <c r="R14" s="31"/>
+      <c r="S14" s="26">
+        <v>31.73</v>
+      </c>
+      <c r="T14" s="26"/>
+      <c r="U14" s="24">
+        <v>32.82</v>
+      </c>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="10">
+        <f>AVERAGE(U14:W14)</f>
+        <v>32.82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="21">
+        <v>90</v>
+      </c>
+      <c r="D15" s="21">
+        <v>60</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1029,21 +1502,55 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="M15" s="6">
+        <v>120</v>
+      </c>
       <c r="N15" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O15" s="13" t="e">
+      <c r="O15" s="13">
         <f t="shared" ref="O15:O21" si="1">AVERAGE(C15:E15)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>2</v>
+      </c>
+      <c r="R15" s="32"/>
+      <c r="S15" s="25">
+        <v>48.21</v>
+      </c>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25">
+        <v>47.87</v>
+      </c>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG15" s="13">
+        <f>AVERAGE(S15:W15)</f>
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="21">
+        <v>30</v>
+      </c>
+      <c r="D16" s="21">
+        <v>30</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1052,23 +1559,55 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="M16" s="6">
+        <v>60</v>
+      </c>
       <c r="N16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="13" t="e">
+      <c r="O16" s="13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>3</v>
+      </c>
+      <c r="R16" s="32"/>
+      <c r="S16" s="25">
+        <v>61.98</v>
+      </c>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25">
+        <v>53.54</v>
+      </c>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG16" s="13">
+        <f>AVERAGE(S16:W16)</f>
+        <v>57.76</v>
+      </c>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C17" s="6">
-        <v>60</v>
-      </c>
-      <c r="D17" s="6"/>
+      <c r="C17" s="21">
+        <v>0</v>
+      </c>
+      <c r="D17" s="21">
+        <v>30</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -1078,22 +1617,56 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="N17" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>4</v>
+      </c>
+      <c r="R17" s="32"/>
+      <c r="S17" s="25">
+        <v>25.09</v>
+      </c>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25">
+        <v>23.33</v>
+      </c>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="AF17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG17" s="13">
+        <f>AVERAGE(S17:W17)</f>
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="3">
         <v>5</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="21">
+        <v>20</v>
+      </c>
+      <c r="D18" s="21">
+        <v>30</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1102,30 +1675,82 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
+      <c r="M18" s="6">
+        <v>100</v>
+      </c>
       <c r="N18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="O18" s="13" t="e">
+      <c r="O18" s="13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>5</v>
+      </c>
+      <c r="R18" s="32"/>
+      <c r="S18" s="25">
+        <v>18.05</v>
+      </c>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25">
+        <v>20.22</v>
+      </c>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG18" s="13">
+        <f>AVERAGE(S18:W18)</f>
+        <v>19.134999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="3">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="N19" s="12" t="s">
         <v>5</v>
       </c>
@@ -1133,22 +1758,76 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q19" s="3">
+        <v>6</v>
+      </c>
+      <c r="R19" s="32"/>
+      <c r="S19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="X19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG19" s="13" t="e">
+        <f>AVERAGE(S19:W19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B20" s="8">
         <v>7</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="N20" s="15" t="s">
         <v>5</v>
       </c>
@@ -1156,8 +1835,40 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q20" s="8">
+        <v>7</v>
+      </c>
+      <c r="R20" s="33"/>
+      <c r="S20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="16" t="e">
+        <f>AVERAGE(S20:W20)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1179,9 +1890,1649 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="Q21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="30"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG21" s="18" t="e">
+        <f>AVERAGE(S21:W21)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="11">
+        <v>46040</v>
+      </c>
+    </row>
+    <row r="24" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>6</v>
+      </c>
+      <c r="I24" s="1">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1">
+        <v>9</v>
+      </c>
+      <c r="L24" s="1">
+        <v>10</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="30"/>
+      <c r="S24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1">
+        <v>2</v>
+      </c>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1">
+        <v>3</v>
+      </c>
+      <c r="X24" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7">
+        <v>60</v>
+      </c>
+      <c r="F25" s="7">
+        <v>50</v>
+      </c>
+      <c r="G25" s="7">
+        <v>50</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7">
+        <v>60</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O25" s="10">
+        <f>AVERAGE(D25:E25)</f>
+        <v>35</v>
+      </c>
+      <c r="P25" s="28">
+        <f>M25-O25</f>
+        <v>25</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>1</v>
+      </c>
+      <c r="R25" s="31"/>
+      <c r="S25" s="23">
+        <v>31.58</v>
+      </c>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23">
+        <v>30.2</v>
+      </c>
+      <c r="V25" s="23"/>
+      <c r="W25" s="7">
+        <v>39.659999999999997</v>
+      </c>
+      <c r="X25" s="7">
+        <v>31.13</v>
+      </c>
+      <c r="Y25" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF25" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="10">
+        <f>AVERAGE(U25:W25)</f>
+        <v>34.93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>90</v>
+      </c>
+      <c r="D26">
+        <v>60</v>
+      </c>
+      <c r="E26" s="6">
+        <v>60</v>
+      </c>
+      <c r="F26" s="6">
+        <v>30</v>
+      </c>
+      <c r="G26" s="6">
+        <v>90</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6">
+        <v>120</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" ref="O26:O32" si="2">AVERAGE(C26:E26)</f>
+        <v>70</v>
+      </c>
+      <c r="P26" s="28">
+        <f t="shared" ref="P26:P29" si="3">M26-O26</f>
+        <v>50</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>2</v>
+      </c>
+      <c r="R26" s="31"/>
+      <c r="S26" s="23">
+        <v>42.4</v>
+      </c>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23">
+        <v>37.44</v>
+      </c>
+      <c r="V26" s="23"/>
+      <c r="W26" s="6">
+        <v>27.12</v>
+      </c>
+      <c r="X26" s="6">
+        <v>27.24</v>
+      </c>
+      <c r="Y26" s="6">
+        <v>25.73</v>
+      </c>
+      <c r="Z26" s="6"/>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG26" s="13">
+        <f>AVERAGE(S26:W26)</f>
+        <v>35.653333333333336</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>60</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+      <c r="G27" s="6">
+        <v>60</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6">
+        <v>60</v>
+      </c>
+      <c r="N27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="P27" s="28">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>3</v>
+      </c>
+      <c r="R27" s="31"/>
+      <c r="S27" s="23">
+        <v>37.42</v>
+      </c>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23">
+        <v>39.729999999999997</v>
+      </c>
+      <c r="V27" s="23"/>
+      <c r="W27" s="6">
+        <v>38.46</v>
+      </c>
+      <c r="X27" s="6">
+        <v>43.48</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>36.130000000000003</v>
+      </c>
+      <c r="Z27" s="6"/>
+      <c r="AA27" s="6"/>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG27" s="13">
+        <f>AVERAGE(S27:W27)</f>
+        <v>38.536666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28" s="6">
+        <v>30</v>
+      </c>
+      <c r="F28" s="6">
+        <v>30</v>
+      </c>
+      <c r="G28" s="6">
+        <v>20</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6">
+        <v>30</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="2"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="P28" s="28">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666679</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>4</v>
+      </c>
+      <c r="R28" s="31"/>
+      <c r="S28" s="23">
+        <v>31.58</v>
+      </c>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23">
+        <v>26.84</v>
+      </c>
+      <c r="V28" s="23"/>
+      <c r="W28" s="6">
+        <v>23.75</v>
+      </c>
+      <c r="X28" s="6">
+        <v>38.92</v>
+      </c>
+      <c r="Y28" s="6">
+        <v>25.52</v>
+      </c>
+      <c r="Z28" s="6"/>
+      <c r="AA28" s="6"/>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="6">
+        <v>60</v>
+      </c>
+      <c r="AF28" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG28" s="13">
+        <f>AVERAGE(S28:W28)</f>
+        <v>27.39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="19">
+        <v>90</v>
+      </c>
+      <c r="D29" s="19">
+        <v>60</v>
+      </c>
+      <c r="E29" s="6">
+        <v>70</v>
+      </c>
+      <c r="F29" s="6">
+        <v>70</v>
+      </c>
+      <c r="G29" s="6">
+        <v>20</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6">
+        <v>100</v>
+      </c>
+      <c r="N29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="2"/>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="P29" s="28">
+        <f t="shared" si="3"/>
+        <v>26.666666666666671</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>5</v>
+      </c>
+      <c r="R29" s="31"/>
+      <c r="S29" s="27">
+        <v>27.2</v>
+      </c>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27">
+        <v>34.5</v>
+      </c>
+      <c r="V29" s="29"/>
+      <c r="W29" s="6">
+        <v>34.770000000000003</v>
+      </c>
+      <c r="X29" s="6">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="Y29" s="6">
+        <v>30.86</v>
+      </c>
+      <c r="Z29" s="6"/>
+      <c r="AA29" s="6"/>
+      <c r="AB29" s="6"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG29" s="13">
+        <f>AVERAGE(S29:W29)</f>
+        <v>32.156666666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="3">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>6</v>
+      </c>
+      <c r="R30" s="32"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG30" s="13" t="e">
+        <f>AVERAGE(S30:W30)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B31" s="8">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="O31" s="16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>7</v>
+      </c>
+      <c r="R31" s="33"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG31" s="16" t="e">
+        <f>AVERAGE(S31:W31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1">
+        <v>70</v>
+      </c>
+      <c r="F32" s="1">
+        <v>70</v>
+      </c>
+      <c r="G32" s="1">
+        <v>70</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O32" s="18">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32" s="30"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG32" s="18" t="e">
+        <f>AVERAGE(S32:W32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B34" s="11">
+        <v>46041</v>
+      </c>
+    </row>
+    <row r="35" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>4</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5</v>
+      </c>
+      <c r="H35" s="1">
+        <v>6</v>
+      </c>
+      <c r="I35" s="1">
+        <v>7</v>
+      </c>
+      <c r="J35" s="1">
+        <v>8</v>
+      </c>
+      <c r="K35" s="1">
+        <v>9</v>
+      </c>
+      <c r="L35" s="1">
+        <v>10</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R35" s="30"/>
+      <c r="S35" s="1">
+        <v>1</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U35" s="1">
+        <v>2</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W35" s="1">
+        <v>3</v>
+      </c>
+      <c r="X35" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC35" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="34">
+        <v>50</v>
+      </c>
+      <c r="D36" s="7">
+        <v>10</v>
+      </c>
+      <c r="E36" s="7">
+        <v>50</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7">
+        <v>60</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O36" s="10">
+        <f>AVERAGE(C36:E36)</f>
+        <v>36.666666666666664</v>
+      </c>
+      <c r="Q36" s="4">
+        <v>1</v>
+      </c>
+      <c r="R36" s="31"/>
+      <c r="S36" s="34">
+        <v>30.28</v>
+      </c>
+      <c r="T36" s="6">
+        <v>19.18</v>
+      </c>
+      <c r="U36" s="7">
+        <v>19.8</v>
+      </c>
+      <c r="V36" s="6">
+        <v>18.27</v>
+      </c>
+      <c r="W36" s="7">
+        <v>27.88</v>
+      </c>
+      <c r="X36" s="7">
+        <v>18.63</v>
+      </c>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF36" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG36" s="10">
+        <f>AVERAGE(S36:W36)</f>
+        <v>23.082000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="6">
+        <v>90</v>
+      </c>
+      <c r="D37" s="6">
+        <v>60</v>
+      </c>
+      <c r="E37" s="6">
+        <v>30</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6">
+        <v>120</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O37" s="13">
+        <f t="shared" ref="O37:O41" si="4">AVERAGE(C37:E37)</f>
+        <v>60</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>2</v>
+      </c>
+      <c r="R37" s="32"/>
+      <c r="S37" s="6">
+        <v>13.91</v>
+      </c>
+      <c r="T37" s="6">
+        <v>11.98</v>
+      </c>
+      <c r="U37" s="6">
+        <v>14.23</v>
+      </c>
+      <c r="V37" s="35">
+        <v>14.26</v>
+      </c>
+      <c r="W37" s="6">
+        <v>10.8</v>
+      </c>
+      <c r="X37" s="6">
+        <v>11.46</v>
+      </c>
+      <c r="Y37" s="6"/>
+      <c r="Z37" s="6"/>
+      <c r="AA37" s="6"/>
+      <c r="AB37" s="6"/>
+      <c r="AC37" s="6"/>
+      <c r="AD37" s="6"/>
+      <c r="AE37" s="6"/>
+      <c r="AF37" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG37" s="13">
+        <f t="shared" ref="AG37:AG42" si="5">AVERAGE(S37:W37)</f>
+        <v>13.036000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6">
+        <v>30</v>
+      </c>
+      <c r="D38" s="6">
+        <v>30</v>
+      </c>
+      <c r="E38" s="6">
+        <v>30</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6">
+        <v>60</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O38" s="13">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>3</v>
+      </c>
+      <c r="R38" s="32"/>
+      <c r="S38" s="6">
+        <v>22.95</v>
+      </c>
+      <c r="T38" s="6">
+        <v>17.75</v>
+      </c>
+      <c r="U38" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="V38" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="W38" s="6">
+        <v>24.08</v>
+      </c>
+      <c r="X38" s="6">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="Y38" s="6"/>
+      <c r="Z38" s="6"/>
+      <c r="AA38" s="6"/>
+      <c r="AB38" s="6"/>
+      <c r="AC38" s="6"/>
+      <c r="AD38" s="6"/>
+      <c r="AE38" s="6"/>
+      <c r="AF38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG38" s="13">
+        <f t="shared" si="5"/>
+        <v>20.756</v>
+      </c>
+    </row>
+    <row r="39" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="3">
+        <v>4</v>
+      </c>
+      <c r="C39" s="6">
+        <v>20</v>
+      </c>
+      <c r="D39" s="6">
+        <v>30</v>
+      </c>
+      <c r="E39" s="6">
+        <v>30</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6">
+        <v>30</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O39" s="13">
+        <f t="shared" si="4"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>4</v>
+      </c>
+      <c r="R39" s="32"/>
+      <c r="S39" s="6">
+        <v>9.01</v>
+      </c>
+      <c r="T39" s="6">
+        <v>12.93</v>
+      </c>
+      <c r="U39" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="V39" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="W39" s="6">
+        <v>10.01</v>
+      </c>
+      <c r="X39" s="6">
+        <v>7.68</v>
+      </c>
+      <c r="Y39" s="6"/>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="6"/>
+      <c r="AB39" s="6"/>
+      <c r="AC39" s="6"/>
+      <c r="AD39" s="6"/>
+      <c r="AE39" s="6">
+        <v>60</v>
+      </c>
+      <c r="AF39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG39" s="13">
+        <f t="shared" si="5"/>
+        <v>10.049999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="3">
+        <v>5</v>
+      </c>
+      <c r="C40" s="6">
+        <v>70</v>
+      </c>
+      <c r="D40" s="6">
+        <v>90</v>
+      </c>
+      <c r="E40" s="6">
+        <v>100</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6">
+        <v>100</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O40" s="13">
+        <f t="shared" si="4"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>5</v>
+      </c>
+      <c r="R40" s="32"/>
+      <c r="S40" s="6">
+        <v>25.22</v>
+      </c>
+      <c r="T40" s="36">
+        <v>0</v>
+      </c>
+      <c r="U40" s="6">
+        <v>27.03</v>
+      </c>
+      <c r="V40" s="36">
+        <v>0</v>
+      </c>
+      <c r="W40" s="6">
+        <v>25.23</v>
+      </c>
+      <c r="X40" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="6"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="6"/>
+      <c r="AB40" s="6"/>
+      <c r="AC40" s="6"/>
+      <c r="AD40" s="6"/>
+      <c r="AE40" s="6"/>
+      <c r="AF40" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG40" s="13">
+        <f t="shared" si="5"/>
+        <v>15.496</v>
+      </c>
+    </row>
+    <row r="41" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B41" s="3"/>
+      <c r="C41" s="6">
+        <v>20</v>
+      </c>
+      <c r="D41" s="6">
+        <v>20</v>
+      </c>
+      <c r="E41" s="6">
+        <v>20</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6">
+        <v>20</v>
+      </c>
+      <c r="N41" s="12"/>
+      <c r="O41" s="13">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="32"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="6"/>
+      <c r="Y41" s="6"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="6"/>
+      <c r="AE41" s="6"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="13"/>
+    </row>
+    <row r="42" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1">
+        <v>50</v>
+      </c>
+      <c r="D42" s="1">
+        <v>35</v>
+      </c>
+      <c r="E42" s="1">
+        <v>50</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="37">
+        <v>50</v>
+      </c>
+      <c r="N42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O42" s="18">
+        <f>AVERAGE(C42:E42)</f>
+        <v>45</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R42" s="30"/>
+      <c r="S42" s="1">
+        <f>SUM(S36:S40)</f>
+        <v>101.37</v>
+      </c>
+      <c r="T42" s="1">
+        <f>SUM(T36:T40)</f>
+        <v>61.839999999999996</v>
+      </c>
+      <c r="U42" s="1">
+        <f t="shared" ref="U42:AD42" si="6">SUM(U36:U40)</f>
+        <v>92.36</v>
+      </c>
+      <c r="V42" s="1">
+        <f t="shared" si="6"/>
+        <v>58.53</v>
+      </c>
+      <c r="W42" s="1">
+        <f t="shared" si="6"/>
+        <v>98</v>
+      </c>
+      <c r="X42" s="1">
+        <f t="shared" si="6"/>
+        <v>57.940000000000005</v>
+      </c>
+      <c r="Y42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG42" s="18"/>
+    </row>
+    <row r="43" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C43">
+        <f>SUM(C36:C42)</f>
+        <v>330</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:L43" si="7">SUM(D36:D42)</f>
+        <v>275</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="7"/>
+        <v>310</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="34">
+        <f>SUM(M36:M42)</f>
+        <v>440</v>
+      </c>
+      <c r="O43" s="38">
+        <f>SUM(O36:O42)</f>
+        <v>305</v>
+      </c>
+      <c r="T43">
+        <f>SUM(S42:T42)</f>
+        <v>163.21</v>
+      </c>
+      <c r="V43">
+        <f>SUM(U42:V42)</f>
+        <v>150.88999999999999</v>
+      </c>
+      <c r="X43">
+        <f>SUM(W42:X42)</f>
+        <v>155.94</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C14:D18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:G29">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C3:M3 O3">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:M10 O3:O10">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:M4 O4">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:M5 O5">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:M7 O7">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:M8 O8">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:M9 O9">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:M10 O10">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:M21 O21">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:M29">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:M32 O32">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:M42 O42">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P25:P29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10:AE10 AG10">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S21:AE21 AG21">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S32:AE32 AG32">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1193,104 +3544,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:M10 O3:O10">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:M4 O4">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:M5 O5">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:M7 O7">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M8 O8">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:M9 O9">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:M10 O10">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:M21 O21">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="S42:AD42 AE43 AG42">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1310,20 +3565,54 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14:V18">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S25:Y29">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:M41">
+    <cfRule type="colorScale" priority="149">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BD7B25-95CA-4382-8A0D-1D65376115BB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Sync from Claire - Wed 01/21/2026 19:36:13.41
</commit_message>
<xml_diff>
--- a/iterations.xlsx
+++ b/iterations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarya\code\FLL-Unearthed-2025---2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\code\FLL-Unearthed-2025---2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C727290-C3EE-459A-9FAA-AFB4486C509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9FF24A-02B0-4E27-8109-6D35E278838B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="12960" windowHeight="7824" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="13">
   <si>
     <t>Run</t>
   </si>
@@ -352,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -416,9 +416,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -430,10 +429,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -776,18 +775,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BA3256-4EE1-4A5D-A5F4-1DDD101D2B98}">
-  <dimension ref="B1:AG43"/>
+  <dimension ref="B1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J13" zoomScale="63" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -795,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -841,7 +840,7 @@
       <c r="Q2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="30"/>
+      <c r="R2" s="29"/>
       <c r="S2" s="1">
         <v>1</v>
       </c>
@@ -884,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -917,7 +916,7 @@
       <c r="Q3" s="4">
         <v>1</v>
       </c>
-      <c r="R3" s="31"/>
+      <c r="R3" s="30"/>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="7"/>
@@ -939,7 +938,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -972,7 +971,7 @@
       <c r="Q4" s="3">
         <v>2</v>
       </c>
-      <c r="R4" s="32"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
@@ -990,11 +989,11 @@
         <v>5</v>
       </c>
       <c r="AG4" s="13" t="e">
-        <f>AVERAGE(S4:W4)</f>
+        <f t="shared" ref="AG4:AG10" si="1">AVERAGE(S4:W4)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -1027,7 +1026,7 @@
       <c r="Q5" s="3">
         <v>3</v>
       </c>
-      <c r="R5" s="32"/>
+      <c r="R5" s="31"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
@@ -1045,11 +1044,11 @@
         <v>5</v>
       </c>
       <c r="AG5" s="13" t="e">
-        <f>AVERAGE(S5:W5)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>4</v>
       </c>
@@ -1082,7 +1081,7 @@
       <c r="Q6" s="3">
         <v>4</v>
       </c>
-      <c r="R6" s="32"/>
+      <c r="R6" s="31"/>
       <c r="S6" s="6">
         <v>60</v>
       </c>
@@ -1104,11 +1103,11 @@
         <v>5</v>
       </c>
       <c r="AG6" s="13">
-        <f>AVERAGE(S6:W6)</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -1141,7 +1140,7 @@
       <c r="Q7" s="3">
         <v>5</v>
       </c>
-      <c r="R7" s="32"/>
+      <c r="R7" s="31"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
@@ -1159,11 +1158,11 @@
         <v>5</v>
       </c>
       <c r="AG7" s="13" t="e">
-        <f>AVERAGE(S7:W7)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -1196,7 +1195,7 @@
       <c r="Q8" s="3">
         <v>6</v>
       </c>
-      <c r="R8" s="32"/>
+      <c r="R8" s="31"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1214,11 +1213,11 @@
         <v>5</v>
       </c>
       <c r="AG8" s="13" t="e">
-        <f>AVERAGE(S8:W8)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -1251,7 +1250,7 @@
       <c r="Q9" s="8">
         <v>7</v>
       </c>
-      <c r="R9" s="33"/>
+      <c r="R9" s="32"/>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
@@ -1269,11 +1268,11 @@
         <v>5</v>
       </c>
       <c r="AG9" s="16" t="e">
-        <f>AVERAGE(S9:W9)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1306,7 +1305,7 @@
       <c r="Q10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="30"/>
+      <c r="R10" s="29"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
@@ -1324,11 +1323,11 @@
         <v>5</v>
       </c>
       <c r="AG10" s="18" t="e">
-        <f>AVERAGE(S10:W10)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +1335,7 @@
         <v>46037</v>
       </c>
     </row>
-    <row r="13" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="5" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1381,7 @@
       <c r="Q13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R13" s="30"/>
+      <c r="R13" s="29"/>
       <c r="S13" s="1">
         <v>1</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>1</v>
       </c>
@@ -1456,7 +1455,7 @@
       <c r="Q14" s="4">
         <v>1</v>
       </c>
-      <c r="R14" s="31"/>
+      <c r="R14" s="30"/>
       <c r="S14" s="26">
         <v>31.73</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>32.82</v>
       </c>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>2</v>
       </c>
@@ -1509,13 +1508,13 @@
         <v>5</v>
       </c>
       <c r="O15" s="13">
-        <f t="shared" ref="O15:O21" si="1">AVERAGE(C15:E15)</f>
+        <f t="shared" ref="O15:O21" si="2">AVERAGE(C15:E15)</f>
         <v>75</v>
       </c>
       <c r="Q15" s="3">
         <v>2</v>
       </c>
-      <c r="R15" s="32"/>
+      <c r="R15" s="31"/>
       <c r="S15" s="25">
         <v>48.21</v>
       </c>
@@ -1537,11 +1536,11 @@
         <v>5</v>
       </c>
       <c r="AG15" s="13">
-        <f>AVERAGE(S15:W15)</f>
+        <f t="shared" ref="AG15:AG21" si="3">AVERAGE(S15:W15)</f>
         <v>48.04</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>3</v>
       </c>
@@ -1566,13 +1565,13 @@
         <v>5</v>
       </c>
       <c r="O16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="Q16" s="3">
         <v>3</v>
       </c>
-      <c r="R16" s="32"/>
+      <c r="R16" s="31"/>
       <c r="S16" s="25">
         <v>61.98</v>
       </c>
@@ -1594,11 +1593,11 @@
         <v>5</v>
       </c>
       <c r="AG16" s="13">
-        <f>AVERAGE(S16:W16)</f>
+        <f t="shared" si="3"/>
         <v>57.76</v>
       </c>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>4</v>
       </c>
@@ -1623,13 +1622,13 @@
         <v>5</v>
       </c>
       <c r="O17" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="Q17" s="3">
         <v>4</v>
       </c>
-      <c r="R17" s="32"/>
+      <c r="R17" s="31"/>
       <c r="S17" s="25">
         <v>25.09</v>
       </c>
@@ -1653,11 +1652,11 @@
         <v>5</v>
       </c>
       <c r="AG17" s="13">
-        <f>AVERAGE(S17:W17)</f>
+        <f t="shared" si="3"/>
         <v>24.21</v>
       </c>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>5</v>
       </c>
@@ -1682,13 +1681,13 @@
         <v>5</v>
       </c>
       <c r="O18" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="Q18" s="3">
         <v>5</v>
       </c>
-      <c r="R18" s="32"/>
+      <c r="R18" s="31"/>
       <c r="S18" s="25">
         <v>18.05</v>
       </c>
@@ -1710,11 +1709,11 @@
         <v>5</v>
       </c>
       <c r="AG18" s="13">
-        <f>AVERAGE(S18:W18)</f>
+        <f t="shared" si="3"/>
         <v>19.134999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>6</v>
       </c>
@@ -1755,13 +1754,13 @@
         <v>5</v>
       </c>
       <c r="O19" s="13" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="3">
         <v>6</v>
       </c>
-      <c r="R19" s="32"/>
+      <c r="R19" s="31"/>
       <c r="S19" s="6" t="s">
         <v>9</v>
       </c>
@@ -1787,11 +1786,11 @@
         <v>5</v>
       </c>
       <c r="AG19" s="13" t="e">
-        <f>AVERAGE(S19:W19)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="8">
         <v>7</v>
       </c>
@@ -1832,13 +1831,13 @@
         <v>5</v>
       </c>
       <c r="O20" s="16" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="8">
         <v>7</v>
       </c>
-      <c r="R20" s="33"/>
+      <c r="R20" s="32"/>
       <c r="S20" s="9" t="s">
         <v>9</v>
       </c>
@@ -1864,11 +1863,11 @@
         <v>5</v>
       </c>
       <c r="AG20" s="16" t="e">
-        <f>AVERAGE(S20:W20)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1887,13 +1886,13 @@
         <v>5</v>
       </c>
       <c r="O21" s="18" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R21" s="30"/>
+      <c r="R21" s="29"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1911,11 +1910,11 @@
         <v>5</v>
       </c>
       <c r="AG21" s="18" t="e">
-        <f>AVERAGE(S21:W21)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>46040</v>
       </c>
     </row>
-    <row r="24" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="5" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +1968,7 @@
       <c r="Q24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R24" s="30"/>
+      <c r="R24" s="29"/>
       <c r="S24" s="1">
         <v>1</v>
       </c>
@@ -2012,7 +2011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>1</v>
       </c>
@@ -2053,7 +2052,7 @@
       <c r="Q25" s="4">
         <v>1</v>
       </c>
-      <c r="R25" s="31"/>
+      <c r="R25" s="30"/>
       <c r="S25" s="23">
         <v>31.58</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>34.93</v>
       </c>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>2</v>
       </c>
@@ -2118,17 +2117,17 @@
         <v>5</v>
       </c>
       <c r="O26" s="13">
-        <f t="shared" ref="O26:O32" si="2">AVERAGE(C26:E26)</f>
+        <f t="shared" ref="O26:O32" si="4">AVERAGE(C26:E26)</f>
         <v>70</v>
       </c>
       <c r="P26" s="28">
-        <f t="shared" ref="P26:P29" si="3">M26-O26</f>
+        <f t="shared" ref="P26:P29" si="5">M26-O26</f>
         <v>50</v>
       </c>
       <c r="Q26" s="3">
         <v>2</v>
       </c>
-      <c r="R26" s="31"/>
+      <c r="R26" s="30"/>
       <c r="S26" s="23">
         <v>42.4</v>
       </c>
@@ -2156,11 +2155,11 @@
         <v>5</v>
       </c>
       <c r="AG26" s="13">
-        <f>AVERAGE(S26:W26)</f>
+        <f t="shared" ref="AG26:AG32" si="6">AVERAGE(S26:W26)</f>
         <v>35.653333333333336</v>
       </c>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>3</v>
       </c>
@@ -2191,17 +2190,17 @@
         <v>5</v>
       </c>
       <c r="O27" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="P27" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="Q27" s="3">
         <v>3</v>
       </c>
-      <c r="R27" s="31"/>
+      <c r="R27" s="30"/>
       <c r="S27" s="23">
         <v>37.42</v>
       </c>
@@ -2229,11 +2228,11 @@
         <v>5</v>
       </c>
       <c r="AG27" s="13">
-        <f>AVERAGE(S27:W27)</f>
+        <f t="shared" si="6"/>
         <v>38.536666666666669</v>
       </c>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>4</v>
       </c>
@@ -2264,17 +2263,17 @@
         <v>5</v>
       </c>
       <c r="O28" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23.333333333333332</v>
       </c>
       <c r="P28" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.6666666666666679</v>
       </c>
       <c r="Q28" s="3">
         <v>4</v>
       </c>
-      <c r="R28" s="31"/>
+      <c r="R28" s="30"/>
       <c r="S28" s="23">
         <v>31.58</v>
       </c>
@@ -2304,11 +2303,11 @@
         <v>5</v>
       </c>
       <c r="AG28" s="13">
-        <f>AVERAGE(S28:W28)</f>
+        <f t="shared" si="6"/>
         <v>27.39</v>
       </c>
     </row>
-    <row r="29" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3">
         <v>5</v>
       </c>
@@ -2339,17 +2338,17 @@
         <v>5</v>
       </c>
       <c r="O29" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>73.333333333333329</v>
       </c>
       <c r="P29" s="28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>26.666666666666671</v>
       </c>
       <c r="Q29" s="3">
         <v>5</v>
       </c>
-      <c r="R29" s="31"/>
+      <c r="R29" s="30"/>
       <c r="S29" s="27">
         <v>27.2</v>
       </c>
@@ -2357,7 +2356,7 @@
       <c r="U29" s="27">
         <v>34.5</v>
       </c>
-      <c r="V29" s="29"/>
+      <c r="V29" s="23"/>
       <c r="W29" s="6">
         <v>34.770000000000003</v>
       </c>
@@ -2377,11 +2376,11 @@
         <v>5</v>
       </c>
       <c r="AG29" s="13">
-        <f>AVERAGE(S29:W29)</f>
+        <f t="shared" si="6"/>
         <v>32.156666666666666</v>
       </c>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>6</v>
       </c>
@@ -2422,13 +2421,13 @@
         <v>5</v>
       </c>
       <c r="O30" s="13" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="3">
         <v>6</v>
       </c>
-      <c r="R30" s="32"/>
+      <c r="R30" s="31"/>
       <c r="S30" s="6"/>
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
@@ -2446,11 +2445,11 @@
         <v>5</v>
       </c>
       <c r="AG30" s="13" t="e">
-        <f>AVERAGE(S30:W30)</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="31" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="8">
         <v>7</v>
       </c>
@@ -2491,13 +2490,13 @@
         <v>5</v>
       </c>
       <c r="O31" s="16" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="8">
         <v>7</v>
       </c>
-      <c r="R31" s="33"/>
+      <c r="R31" s="32"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>
@@ -2515,11 +2514,11 @@
         <v>5</v>
       </c>
       <c r="AG31" s="16" t="e">
-        <f>AVERAGE(S31:W31)</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="32" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="5" t="s">
         <v>3</v>
       </c>
@@ -2544,13 +2543,13 @@
         <v>5</v>
       </c>
       <c r="O32" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="Q32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R32" s="30"/>
+      <c r="R32" s="29"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -2568,16 +2567,16 @@
         <v>5</v>
       </c>
       <c r="AG32" s="18" t="e">
-        <f>AVERAGE(S32:W32)</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="34" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="11">
         <v>46041</v>
       </c>
     </row>
-    <row r="35" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="35" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="5" t="s">
         <v>0</v>
       </c>
@@ -2623,7 +2622,7 @@
       <c r="Q35" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R35" s="30"/>
+      <c r="R35" s="29"/>
       <c r="S35" s="1">
         <v>1</v>
       </c>
@@ -2670,11 +2669,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <v>1</v>
       </c>
-      <c r="C36" s="34">
+      <c r="C36" s="33">
         <v>50</v>
       </c>
       <c r="D36" s="7">
@@ -2703,8 +2702,8 @@
       <c r="Q36" s="4">
         <v>1</v>
       </c>
-      <c r="R36" s="31"/>
-      <c r="S36" s="34">
+      <c r="R36" s="30"/>
+      <c r="S36" s="33">
         <v>30.28</v>
       </c>
       <c r="T36" s="6">
@@ -2739,7 +2738,7 @@
         <v>23.082000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B37" s="3">
         <v>2</v>
       </c>
@@ -2766,13 +2765,13 @@
         <v>5</v>
       </c>
       <c r="O37" s="13">
-        <f t="shared" ref="O37:O41" si="4">AVERAGE(C37:E37)</f>
+        <f t="shared" ref="O37:O41" si="7">AVERAGE(C37:E37)</f>
         <v>60</v>
       </c>
       <c r="Q37" s="3">
         <v>2</v>
       </c>
-      <c r="R37" s="32"/>
+      <c r="R37" s="31"/>
       <c r="S37" s="6">
         <v>13.91</v>
       </c>
@@ -2782,7 +2781,7 @@
       <c r="U37" s="6">
         <v>14.23</v>
       </c>
-      <c r="V37" s="35">
+      <c r="V37" s="34">
         <v>14.26</v>
       </c>
       <c r="W37" s="6">
@@ -2802,11 +2801,11 @@
         <v>5</v>
       </c>
       <c r="AG37" s="13">
-        <f t="shared" ref="AG37:AG42" si="5">AVERAGE(S37:W37)</f>
+        <f t="shared" ref="AG37:AG40" si="8">AVERAGE(S37:W37)</f>
         <v>13.036000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B38" s="3">
         <v>3</v>
       </c>
@@ -2833,13 +2832,13 @@
         <v>5</v>
       </c>
       <c r="O38" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="Q38" s="3">
         <v>3</v>
       </c>
-      <c r="R38" s="32"/>
+      <c r="R38" s="31"/>
       <c r="S38" s="6">
         <v>22.95</v>
       </c>
@@ -2869,11 +2868,11 @@
         <v>5</v>
       </c>
       <c r="AG38" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>20.756</v>
       </c>
     </row>
-    <row r="39" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B39" s="3">
         <v>4</v>
       </c>
@@ -2900,13 +2899,13 @@
         <v>5</v>
       </c>
       <c r="O39" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>26.666666666666668</v>
       </c>
       <c r="Q39" s="3">
         <v>4</v>
       </c>
-      <c r="R39" s="32"/>
+      <c r="R39" s="31"/>
       <c r="S39" s="6">
         <v>9.01</v>
       </c>
@@ -2938,11 +2937,11 @@
         <v>5</v>
       </c>
       <c r="AG39" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10.049999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B40" s="3">
         <v>5</v>
       </c>
@@ -2969,23 +2968,23 @@
         <v>5</v>
       </c>
       <c r="O40" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>86.666666666666671</v>
       </c>
       <c r="Q40" s="3">
         <v>5</v>
       </c>
-      <c r="R40" s="32"/>
+      <c r="R40" s="31"/>
       <c r="S40" s="6">
         <v>25.22</v>
       </c>
-      <c r="T40" s="36">
+      <c r="T40" s="35">
         <v>0</v>
       </c>
       <c r="U40" s="6">
         <v>27.03</v>
       </c>
-      <c r="V40" s="36">
+      <c r="V40" s="35">
         <v>0</v>
       </c>
       <c r="W40" s="6">
@@ -3005,11 +3004,11 @@
         <v>5</v>
       </c>
       <c r="AG40" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15.496</v>
       </c>
     </row>
-    <row r="41" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="41" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B41" s="3"/>
       <c r="C41" s="6">
         <v>20</v>
@@ -3032,11 +3031,11 @@
       </c>
       <c r="N41" s="12"/>
       <c r="O41" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="Q41" s="3"/>
-      <c r="R41" s="32"/>
+      <c r="R41" s="31"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
@@ -3053,7 +3052,7 @@
       <c r="AF41" s="12"/>
       <c r="AG41" s="13"/>
     </row>
-    <row r="42" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="42" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
@@ -3073,7 +3072,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="37">
+      <c r="M42" s="36">
         <v>50</v>
       </c>
       <c r="N42" s="17" t="s">
@@ -3086,7 +3085,7 @@
       <c r="Q42" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R42" s="30"/>
+      <c r="R42" s="29"/>
       <c r="S42" s="1">
         <f>SUM(S36:S40)</f>
         <v>101.37</v>
@@ -3096,43 +3095,43 @@
         <v>61.839999999999996</v>
       </c>
       <c r="U42" s="1">
-        <f t="shared" ref="U42:AD42" si="6">SUM(U36:U40)</f>
+        <f t="shared" ref="U42:AD42" si="9">SUM(U36:U40)</f>
         <v>92.36</v>
       </c>
       <c r="V42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>58.53</v>
       </c>
       <c r="W42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>98</v>
       </c>
       <c r="X42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>57.940000000000005</v>
       </c>
       <c r="Y42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AC42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AD42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AF42" s="17" t="s">
@@ -3140,52 +3139,52 @@
       </c>
       <c r="AG42" s="18"/>
     </row>
-    <row r="43" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="43" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C43">
         <f>SUM(C36:C42)</f>
         <v>330</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:L43" si="7">SUM(D36:D42)</f>
+        <f t="shared" ref="D43:L43" si="10">SUM(D36:D42)</f>
         <v>275</v>
       </c>
       <c r="E43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>310</v>
       </c>
       <c r="F43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L43">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="33">
         <f>SUM(M36:M42)</f>
         <v>440</v>
       </c>
-      <c r="O43" s="38">
+      <c r="O43" s="37">
         <f>SUM(O36:O42)</f>
         <v>305</v>
       </c>
@@ -3205,9 +3204,642 @@
         <v>150</v>
       </c>
     </row>
+    <row r="47" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="11">
+        <v>46043</v>
+      </c>
+    </row>
+    <row r="48" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1">
+        <v>3</v>
+      </c>
+      <c r="F48" s="1">
+        <v>4</v>
+      </c>
+      <c r="G48" s="1">
+        <v>5</v>
+      </c>
+      <c r="H48" s="1">
+        <v>6</v>
+      </c>
+      <c r="I48" s="1">
+        <v>7</v>
+      </c>
+      <c r="J48" s="1">
+        <v>8</v>
+      </c>
+      <c r="K48" s="1">
+        <v>9</v>
+      </c>
+      <c r="L48" s="1">
+        <v>10</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R48" s="29"/>
+      <c r="S48" s="1">
+        <v>1</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U48" s="1">
+        <v>2</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W48" s="1">
+        <v>3</v>
+      </c>
+      <c r="X48" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y48" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB48" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC48" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD48" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG48" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="33">
+        <v>50</v>
+      </c>
+      <c r="D49" s="7">
+        <v>10</v>
+      </c>
+      <c r="E49" s="7">
+        <v>50</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7">
+        <v>60</v>
+      </c>
+      <c r="N49" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O49" s="10">
+        <f>AVERAGE(C49:E49)</f>
+        <v>36.666666666666664</v>
+      </c>
+      <c r="Q49" s="4">
+        <v>1</v>
+      </c>
+      <c r="R49" s="30"/>
+      <c r="S49" s="33">
+        <v>30.28</v>
+      </c>
+      <c r="T49" s="6">
+        <v>19.18</v>
+      </c>
+      <c r="U49" s="7">
+        <v>19.8</v>
+      </c>
+      <c r="V49" s="6">
+        <v>18.27</v>
+      </c>
+      <c r="W49" s="7">
+        <v>27.88</v>
+      </c>
+      <c r="X49" s="7">
+        <v>18.63</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7"/>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7"/>
+      <c r="AC49" s="7"/>
+      <c r="AD49" s="7"/>
+      <c r="AE49" s="7">
+        <v>60</v>
+      </c>
+      <c r="AF49" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG49" s="10">
+        <f>AVERAGE(S49:W49)</f>
+        <v>23.082000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B50" s="3">
+        <v>2</v>
+      </c>
+      <c r="C50" s="6">
+        <v>90</v>
+      </c>
+      <c r="D50" s="6">
+        <v>60</v>
+      </c>
+      <c r="E50" s="6">
+        <v>30</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6">
+        <v>120</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O50" s="13">
+        <f t="shared" ref="O50:O54" si="11">AVERAGE(C50:E50)</f>
+        <v>60</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>2</v>
+      </c>
+      <c r="R50" s="31"/>
+      <c r="S50" s="6">
+        <v>13.91</v>
+      </c>
+      <c r="T50" s="6">
+        <v>11.98</v>
+      </c>
+      <c r="U50" s="6">
+        <v>14.23</v>
+      </c>
+      <c r="V50" s="34">
+        <v>14.26</v>
+      </c>
+      <c r="W50" s="6">
+        <v>10.8</v>
+      </c>
+      <c r="X50" s="6">
+        <v>11.46</v>
+      </c>
+      <c r="Y50" s="6"/>
+      <c r="Z50" s="6"/>
+      <c r="AA50" s="6"/>
+      <c r="AB50" s="6"/>
+      <c r="AC50" s="6"/>
+      <c r="AD50" s="6"/>
+      <c r="AE50" s="6"/>
+      <c r="AF50" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG50" s="13">
+        <f t="shared" ref="AG50:AG53" si="12">AVERAGE(S50:W50)</f>
+        <v>13.036000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B51" s="3">
+        <v>3</v>
+      </c>
+      <c r="C51" s="6">
+        <v>30</v>
+      </c>
+      <c r="D51" s="6">
+        <v>30</v>
+      </c>
+      <c r="E51" s="6">
+        <v>30</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6">
+        <v>60</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O51" s="13">
+        <f t="shared" si="11"/>
+        <v>30</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>3</v>
+      </c>
+      <c r="R51" s="31"/>
+      <c r="S51" s="6">
+        <v>22.95</v>
+      </c>
+      <c r="T51" s="6">
+        <v>17.75</v>
+      </c>
+      <c r="U51" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="V51" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="W51" s="6">
+        <v>24.08</v>
+      </c>
+      <c r="X51" s="6">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="Y51" s="6"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="6"/>
+      <c r="AB51" s="6"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="6"/>
+      <c r="AF51" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG51" s="13">
+        <f t="shared" si="12"/>
+        <v>20.756</v>
+      </c>
+    </row>
+    <row r="52" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B52" s="3">
+        <v>4</v>
+      </c>
+      <c r="C52" s="6">
+        <v>20</v>
+      </c>
+      <c r="D52" s="6">
+        <v>30</v>
+      </c>
+      <c r="E52" s="6">
+        <v>30</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6">
+        <v>30</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O52" s="13">
+        <f t="shared" si="11"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>4</v>
+      </c>
+      <c r="R52" s="31"/>
+      <c r="S52" s="6">
+        <v>9.01</v>
+      </c>
+      <c r="T52" s="6">
+        <v>12.93</v>
+      </c>
+      <c r="U52" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="V52" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="W52" s="6">
+        <v>10.01</v>
+      </c>
+      <c r="X52" s="6">
+        <v>7.68</v>
+      </c>
+      <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="6"/>
+      <c r="AB52" s="6"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="6">
+        <v>60</v>
+      </c>
+      <c r="AF52" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG52" s="13">
+        <f t="shared" si="12"/>
+        <v>10.049999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="C53" s="6">
+        <v>70</v>
+      </c>
+      <c r="D53" s="6">
+        <v>90</v>
+      </c>
+      <c r="E53" s="6">
+        <v>100</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6">
+        <v>100</v>
+      </c>
+      <c r="N53" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O53" s="13">
+        <f t="shared" si="11"/>
+        <v>86.666666666666671</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>5</v>
+      </c>
+      <c r="R53" s="31"/>
+      <c r="S53" s="6">
+        <v>25.22</v>
+      </c>
+      <c r="T53" s="35">
+        <v>0</v>
+      </c>
+      <c r="U53" s="6">
+        <v>27.03</v>
+      </c>
+      <c r="V53" s="35">
+        <v>0</v>
+      </c>
+      <c r="W53" s="6">
+        <v>25.23</v>
+      </c>
+      <c r="X53" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="6"/>
+      <c r="AB53" s="6"/>
+      <c r="AC53" s="6"/>
+      <c r="AD53" s="6"/>
+      <c r="AE53" s="6"/>
+      <c r="AF53" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG53" s="13">
+        <f t="shared" si="12"/>
+        <v>15.496</v>
+      </c>
+    </row>
+    <row r="54" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="3"/>
+      <c r="C54" s="6">
+        <v>20</v>
+      </c>
+      <c r="D54" s="6">
+        <v>20</v>
+      </c>
+      <c r="E54" s="6">
+        <v>20</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6">
+        <v>20</v>
+      </c>
+      <c r="N54" s="12"/>
+      <c r="O54" s="13">
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+      <c r="X54" s="6"/>
+      <c r="Y54" s="6"/>
+      <c r="Z54" s="6"/>
+      <c r="AA54" s="6"/>
+      <c r="AB54" s="6"/>
+      <c r="AC54" s="6"/>
+      <c r="AD54" s="6"/>
+      <c r="AE54" s="6"/>
+      <c r="AF54" s="12"/>
+      <c r="AG54" s="13"/>
+    </row>
+    <row r="55" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="1">
+        <v>50</v>
+      </c>
+      <c r="D55" s="1">
+        <v>35</v>
+      </c>
+      <c r="E55" s="1">
+        <v>50</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="36">
+        <v>50</v>
+      </c>
+      <c r="N55" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="O55" s="18">
+        <f>AVERAGE(C55:E55)</f>
+        <v>45</v>
+      </c>
+      <c r="Q55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R55" s="29"/>
+      <c r="S55" s="1">
+        <f>SUM(S49:S53)</f>
+        <v>101.37</v>
+      </c>
+      <c r="T55" s="1">
+        <f>SUM(T49:T53)</f>
+        <v>61.839999999999996</v>
+      </c>
+      <c r="U55" s="1">
+        <f t="shared" ref="U55:AD55" si="13">SUM(U49:U53)</f>
+        <v>92.36</v>
+      </c>
+      <c r="V55" s="1">
+        <f t="shared" si="13"/>
+        <v>58.53</v>
+      </c>
+      <c r="W55" s="1">
+        <f t="shared" si="13"/>
+        <v>98</v>
+      </c>
+      <c r="X55" s="1">
+        <f t="shared" si="13"/>
+        <v>57.940000000000005</v>
+      </c>
+      <c r="Y55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Z55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AA55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AB55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AC55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD55" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AF55" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG55" s="18"/>
+    </row>
+    <row r="56" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C56">
+        <f>SUM(C49:C55)</f>
+        <v>330</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ref="D56:L56" si="14">SUM(D49:D55)</f>
+        <v>275</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="14"/>
+        <v>310</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="33">
+        <f>SUM(M49:M55)</f>
+        <v>440</v>
+      </c>
+      <c r="O56" s="37">
+        <f>SUM(O49:O55)</f>
+        <v>305</v>
+      </c>
+      <c r="T56">
+        <f>SUM(S55:T55)</f>
+        <v>163.21</v>
+      </c>
+      <c r="V56">
+        <f>SUM(U55:V55)</f>
+        <v>150.88999999999999</v>
+      </c>
+      <c r="X56">
+        <f>SUM(W55:X55)</f>
+        <v>155.94</v>
+      </c>
+      <c r="AE56" s="1">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C14:D18">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3219,7 +3851,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:G29">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3231,7 +3863,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M3 O3">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3243,6 +3875,90 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M10 O3:O10">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:M4 O4">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:M5 O5">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:M7 O7">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:M8 O8">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:M9 O9">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:M10 O10">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -3254,92 +3970,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:M4 O4">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:M5 O5">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:M7 O7">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:M8 O8">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:M9 O9">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:M10 C21:M21 O21 O10">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:M10 O10">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21 O21">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3361,7 +3993,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:M29">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3373,7 +4005,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:M32 O32">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3383,6 +4015,40 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:M41">
+    <cfRule type="colorScale" priority="156">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42:M42 O42">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3403,29 +4069,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:M42 O42">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3437,7 +4081,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25:P29">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3448,8 +4092,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10:AE10 AG10">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="S14:V18">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S25:Y29">
+    <cfRule type="colorScale" priority="128">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S42:AD42 AE43 AG42">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3459,7 +4127,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3469,7 +4137,39 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10:AE10 AG10">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3481,7 +4181,49 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S21:AE21 AG21">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S32:AE32 AG32">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3501,7 +4243,9 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="22">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:M54">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3512,8 +4256,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S32:AE32 AG32">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="C55:M55 O55">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3523,7 +4267,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3533,7 +4277,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3544,8 +4288,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S42:AD42 AE43 AG42">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="S55:AD55 AE56 AG55">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3555,7 +4299,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3565,43 +4309,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S14:V18">
-    <cfRule type="colorScale" priority="70">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S25:Y29">
-    <cfRule type="colorScale" priority="121">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36:M41">
-    <cfRule type="colorScale" priority="149">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Sync from Mermaid-Harry - Fri 01/23/2026 18:20:19.97
</commit_message>
<xml_diff>
--- a/iterations.xlsx
+++ b/iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarya\code\FLL-Unearthed-2025---2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDE8472-4119-48F8-855D-56D2CFBFE440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7869A65A-2F08-4B2B-A175-6DEBDF6494C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{14DBA40A-3910-463C-AF80-11027D66D5E7}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="15">
   <si>
     <t>Run</t>
   </si>
@@ -84,6 +84,9 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>extension</t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -485,27 +488,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -846,7 +839,7 @@
   <dimension ref="B1:AG56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="63" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3328,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="T48" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U48" s="1">
         <v>2</v>
@@ -3377,8 +3370,12 @@
       <c r="C49" s="33">
         <v>60</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
+      <c r="D49" s="7">
+        <v>50</v>
+      </c>
+      <c r="E49" s="7">
+        <v>60</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -3394,7 +3391,7 @@
       </c>
       <c r="O49" s="10">
         <f>AVERAGE(C49:E49)</f>
-        <v>60</v>
+        <v>56.666666666666664</v>
       </c>
       <c r="Q49" s="4">
         <v>1</v>
@@ -3406,10 +3403,18 @@
       <c r="T49" s="41">
         <v>18</v>
       </c>
-      <c r="U49" s="41"/>
-      <c r="V49" s="41"/>
-      <c r="W49" s="41"/>
-      <c r="X49" s="41"/>
+      <c r="U49" s="41">
+        <v>30.28</v>
+      </c>
+      <c r="V49" s="41">
+        <v>19.829999999999998</v>
+      </c>
+      <c r="W49" s="41">
+        <v>30.15</v>
+      </c>
+      <c r="X49" s="41">
+        <v>19.829999999999998</v>
+      </c>
       <c r="Y49" s="7"/>
       <c r="Z49" s="7"/>
       <c r="AA49" s="7"/>
@@ -3424,7 +3429,7 @@
       </c>
       <c r="AG49" s="10">
         <f>AVERAGE(S49:W49)</f>
-        <v>24.5</v>
+        <v>25.851999999999997</v>
       </c>
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.55000000000000004">
@@ -3434,8 +3439,12 @@
       <c r="C50" s="6">
         <v>90</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="D50" s="6">
+        <v>120</v>
+      </c>
+      <c r="E50" s="6">
+        <v>120</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -3451,7 +3460,7 @@
       </c>
       <c r="O50" s="13">
         <f t="shared" ref="O50:O54" si="11">AVERAGE(C50:E50)</f>
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="Q50" s="3">
         <v>2</v>
@@ -3463,10 +3472,18 @@
       <c r="T50" s="39">
         <v>16</v>
       </c>
-      <c r="U50" s="39"/>
-      <c r="V50" s="39"/>
-      <c r="W50" s="39"/>
-      <c r="X50" s="39"/>
+      <c r="U50" s="39">
+        <v>17.73</v>
+      </c>
+      <c r="V50" s="39">
+        <v>17.03</v>
+      </c>
+      <c r="W50" s="39">
+        <v>18.28</v>
+      </c>
+      <c r="X50" s="39">
+        <v>16.36</v>
+      </c>
       <c r="Y50" s="6"/>
       <c r="Z50" s="6"/>
       <c r="AA50" s="6"/>
@@ -3479,7 +3496,7 @@
       </c>
       <c r="AG50" s="13">
         <f t="shared" ref="AG50:AG53" si="12">AVERAGE(S50:W50)</f>
-        <v>16</v>
+        <v>17.260000000000002</v>
       </c>
     </row>
     <row r="51" spans="2:33" x14ac:dyDescent="0.55000000000000004">
@@ -3489,8 +3506,12 @@
       <c r="C51" s="6">
         <v>30</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="D51" s="6">
+        <v>30</v>
+      </c>
+      <c r="E51" s="6">
+        <v>50</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -3506,7 +3527,7 @@
       </c>
       <c r="O51" s="13">
         <f t="shared" si="11"/>
-        <v>30</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="Q51" s="3">
         <v>3</v>
@@ -3518,10 +3539,18 @@
       <c r="T51" s="39">
         <v>23</v>
       </c>
-      <c r="U51" s="39"/>
-      <c r="V51" s="39"/>
-      <c r="W51" s="39"/>
-      <c r="X51" s="39"/>
+      <c r="U51" s="39">
+        <v>19.82</v>
+      </c>
+      <c r="V51" s="39">
+        <v>18.37</v>
+      </c>
+      <c r="W51" s="39">
+        <v>27.2</v>
+      </c>
+      <c r="X51" s="39">
+        <v>18.45</v>
+      </c>
       <c r="Y51" s="6"/>
       <c r="Z51" s="6"/>
       <c r="AA51" s="6"/>
@@ -3534,7 +3563,7 @@
       </c>
       <c r="AG51" s="13">
         <f t="shared" si="12"/>
-        <v>20.5</v>
+        <v>21.277999999999999</v>
       </c>
     </row>
     <row r="52" spans="2:33" x14ac:dyDescent="0.55000000000000004">
@@ -3544,8 +3573,12 @@
       <c r="C52" s="6">
         <v>40</v>
       </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="D52" s="6">
+        <v>30</v>
+      </c>
+      <c r="E52" s="6">
+        <v>40</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -3554,14 +3587,14 @@
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="44">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N52" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O52" s="13">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="Q52" s="3">
         <v>4</v>
@@ -3573,10 +3606,18 @@
       <c r="T52" s="39">
         <v>9.91</v>
       </c>
-      <c r="U52" s="39"/>
-      <c r="V52" s="39"/>
-      <c r="W52" s="39"/>
-      <c r="X52" s="39"/>
+      <c r="U52" s="39">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="V52" s="39">
+        <v>22.92</v>
+      </c>
+      <c r="W52" s="39">
+        <v>8.98</v>
+      </c>
+      <c r="X52" s="39">
+        <v>9.33</v>
+      </c>
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
       <c r="AA52" s="6"/>
@@ -3591,7 +3632,7 @@
       </c>
       <c r="AG52" s="13">
         <f t="shared" si="12"/>
-        <v>9.4550000000000001</v>
+        <v>11.872</v>
       </c>
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.55000000000000004">
@@ -3601,8 +3642,12 @@
       <c r="C53" s="6">
         <v>100</v>
       </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="D53" s="6">
+        <v>40</v>
+      </c>
+      <c r="E53" s="6">
+        <v>30</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
@@ -3618,7 +3663,7 @@
       </c>
       <c r="O53" s="13">
         <f t="shared" si="11"/>
-        <v>100</v>
+        <v>56.666666666666664</v>
       </c>
       <c r="Q53" s="3">
         <v>5</v>
@@ -3630,9 +3675,13 @@
       <c r="T53" s="39">
         <v>0</v>
       </c>
-      <c r="U53" s="39"/>
+      <c r="U53" s="39">
+        <v>21.6</v>
+      </c>
       <c r="V53" s="39"/>
-      <c r="W53" s="39"/>
+      <c r="W53" s="39">
+        <v>20.87</v>
+      </c>
       <c r="X53" s="39"/>
       <c r="Y53" s="6"/>
       <c r="Z53" s="6"/>
@@ -3646,7 +3695,7 @@
       </c>
       <c r="AG53" s="13">
         <f t="shared" si="12"/>
-        <v>11.5</v>
+        <v>16.3675</v>
       </c>
     </row>
     <row r="54" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3705,7 +3754,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="45">
+      <c r="M55" s="36">
         <v>50</v>
       </c>
       <c r="N55" s="17" t="s">
@@ -3727,19 +3776,19 @@
       </c>
       <c r="U55" s="38">
         <f t="shared" ref="U55:AD55" si="13">SUM(U49:U53)</f>
-        <v>0</v>
+        <v>97.980000000000018</v>
       </c>
       <c r="V55" s="38">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>78.150000000000006</v>
       </c>
       <c r="W55" s="38">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>105.48</v>
       </c>
       <c r="X55" s="38">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>63.97</v>
       </c>
       <c r="Y55" s="1">
         <f t="shared" si="13"/>
@@ -3772,48 +3821,48 @@
     </row>
     <row r="56" spans="2:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C56">
-        <f>SUM(C49:C55)</f>
+        <f t="shared" ref="C56:M56" si="14">SUM(C49:C55)</f>
         <v>355</v>
       </c>
       <c r="D56">
-        <f>SUM(D49:D55)</f>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>270</v>
       </c>
       <c r="E56">
-        <f>SUM(E49:E55)</f>
-        <v>50</v>
+        <f t="shared" si="14"/>
+        <v>350</v>
       </c>
       <c r="F56">
-        <f>SUM(F49:F55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G56">
-        <f>SUM(G49:G55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H56">
-        <f>SUM(H49:H55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I56">
-        <f>SUM(I49:I55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J56">
-        <f>SUM(J49:J55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K56">
-        <f>SUM(K49:K55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="L56">
-        <f>SUM(L49:L55)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M56" s="33">
-        <f>SUM(M49:M55)</f>
-        <v>440</v>
+        <f t="shared" si="14"/>
+        <v>450</v>
       </c>
       <c r="O56" s="37" t="e">
         <f>SUM(O49:O55)</f>
@@ -3825,11 +3874,11 @@
       </c>
       <c r="V56">
         <f>SUM(U55:V55)</f>
-        <v>0</v>
+        <v>176.13000000000002</v>
       </c>
       <c r="X56">
         <f>SUM(W55:X55)</f>
-        <v>0</v>
+        <v>169.45</v>
       </c>
       <c r="AE56" s="1">
         <v>150</v>
@@ -3858,6 +3907,11 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:L49">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C49=$M$49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:M3 O3">
@@ -3969,7 +4023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:M21 O21">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3979,7 +4033,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4003,16 +4057,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:M32 O32">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -4024,6 +4068,16 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4047,7 +4101,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:M42 O42">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4067,7 +4121,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4115,7 +4169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S42:AD42 AE43 AG42">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4135,7 +4189,39 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S55:AD55 AE56 AG55">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4179,16 +4265,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S21:AE21 AG21">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -4209,9 +4285,19 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S32:AE32 AG32">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4231,7 +4317,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4242,43 +4328,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S55:AD55 AE56 AG55">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:L49">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>C49=$M$49</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>